<commit_message>
updated and working v0.1
</commit_message>
<xml_diff>
--- a/config/config_single.xlsx
+++ b/config/config_single.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghyun/github/pypsa_alternative/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3CBC8C-27EC-4746-9734-36C55CDBEB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9744CC8-3AD2-904A-A850-FCF5ECC8EECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,7 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1368,7 +1368,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1391,7 +1391,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>0.7</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1483,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
         <v>1</v>

</xml_diff>